<commit_message>
CST-3512 Ticket State Queue Mapping test
</commit_message>
<xml_diff>
--- a/Excels/MG.xlsx
+++ b/Excels/MG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Ticket State" sheetId="10" r:id="rId12"/>
     <sheet name="UserManagement" sheetId="13" r:id="rId13"/>
     <sheet name="TemplateManagement" sheetId="14" r:id="rId14"/>
+    <sheet name="State Queue Mapping" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'FTRTickets-Reg'!$A$1:$F$126</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="901">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="912">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -2744,6 +2745,39 @@
   </si>
   <si>
     <t>Total Committed SLA</t>
+  </si>
+  <si>
+    <t>Queue Name</t>
+  </si>
+  <si>
+    <t>State name1</t>
+  </si>
+  <si>
+    <t>State name2</t>
+  </si>
+  <si>
+    <t>State name3</t>
+  </si>
+  <si>
+    <t>State name4</t>
+  </si>
+  <si>
+    <t>State name5</t>
+  </si>
+  <si>
+    <t>State name6</t>
+  </si>
+  <si>
+    <t>State name7</t>
+  </si>
+  <si>
+    <t>State name8</t>
+  </si>
+  <si>
+    <t>State name9</t>
+  </si>
+  <si>
+    <t>State name10</t>
   </si>
 </sst>
 </file>
@@ -3005,7 +3039,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
@@ -3059,6 +3093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3405,7 +3440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3699,7 +3734,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3940,6 +3975,124 @@
       <c r="A7" s="1" t="s">
         <v>152</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>901</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>902</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>903</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>904</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>905</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>906</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>907</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>908</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>909</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>910</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14147,7 +14300,7 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>